<commit_message>
Update prior to workshop in Tutzing
</commit_message>
<xml_diff>
--- a/Results/Table_3.xlsx
+++ b/Results/Table_3.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\meta_theory\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{5B31B9A3-8436-44C8-9442-D8B12FB0CBBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C1C1178-8E36-496E-8F9D-79EF13AF1365}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table_3" sheetId="1" r:id="rId1"/>
@@ -46,64 +46,129 @@
     <t>Full Model Compatible:</t>
   </si>
   <si>
-    <t>*In lavaan notation, X4 ~ X4 means adjusted but independent</t>
+    <r>
+      <t>Reference Model is Y ~ X</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + X</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, X</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ~ X</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + X</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (Model 1)</t>
+    </r>
   </si>
   <si>
     <r>
-      <t>Reference Model is Y ~ X</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> + X</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>test</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, X</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>test</t>
+      <t>*In lavaan notation, X</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
     </r>
     <r>
       <rPr>
@@ -124,43 +189,85 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> + X</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (Model 1)</t>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> means adjusted but independent</t>
     </r>
   </si>
   <si>
     <r>
-      <t>Multiverse includes models with X</t>
+      <t>Reference Model is Y ~ X</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + X</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, X</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>test</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ~ X</t>
     </r>
     <r>
       <rPr>
@@ -181,7 +288,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> and X</t>
+      <t xml:space="preserve"> + X</t>
     </r>
     <r>
       <rPr>
@@ -202,86 +309,75 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>, and models with X</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>X</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and X</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>4</t>
+      <t>, X</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">3 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>~ X</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>* (Model 7)</t>
     </r>
   </si>
   <si>
     <r>
-      <t>Reference Model is Y ~ X</t>
+      <t>Multiverse Criteria: Models with X</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and X</t>
     </r>
     <r>
       <rPr>
@@ -302,49 +398,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> + X</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>test</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>, X</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>test</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ~ X</t>
+      <t>, and models with X</t>
     </r>
     <r>
       <rPr>
@@ -365,7 +419,28 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> + X</t>
+      <t>,</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>X</t>
     </r>
     <r>
       <rPr>
@@ -386,54 +461,23 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>, X</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">4 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>~ X</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="subscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>* (Model 7)</t>
+      <t xml:space="preserve"> and X</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3</t>
     </r>
   </si>
   <si>
     <r>
-      <t>Multiverse Criteria models with X</t>
+      <t>Multiverse Criteria: Models with X</t>
     </r>
     <r>
       <rPr>
@@ -493,7 +537,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
@@ -1008,7 +1052,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1043,6 +1087,13 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1397,11 +1448,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:I21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:B21"/>
+      <selection activeCell="A2" sqref="A2:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1422,12 +1473,12 @@
     </row>
     <row r="3" spans="1:9" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
@@ -1446,7 +1497,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="12">
-        <v>1087</v>
+        <v>1165</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="5" t="s">
@@ -1461,14 +1512,14 @@
         <v>5</v>
       </c>
       <c r="B7" s="13">
-        <v>0.18099999999999999</v>
+        <v>0.27</v>
       </c>
       <c r="C7" s="2"/>
       <c r="D7" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E7" s="13">
-        <v>0.71899999999999997</v>
+        <v>0.28100000000000003</v>
       </c>
       <c r="G7" s="1"/>
     </row>
@@ -1477,14 +1528,14 @@
         <v>7</v>
       </c>
       <c r="B8" s="16">
-        <v>4.7E-2</v>
+        <v>5.3999999999999999E-2</v>
       </c>
       <c r="C8" s="17"/>
       <c r="D8" s="15" t="s">
         <v>7</v>
       </c>
       <c r="E8" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
@@ -1499,15 +1550,17 @@
     </row>
     <row r="10" spans="1:9" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="I10" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="I10" s="18"/>
     </row>
     <row r="11" spans="1:9" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>12</v>
       </c>
-      <c r="I11" s="5"/>
+      <c r="G11" s="1"/>
+      <c r="I11" s="19"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
@@ -1525,7 +1578,7 @@
         <v>6</v>
       </c>
       <c r="B13" s="12">
-        <v>1087</v>
+        <v>1165</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="5" t="s">
@@ -1540,14 +1593,14 @@
         <v>5</v>
       </c>
       <c r="B14" s="13">
-        <v>0.71899999999999997</v>
+        <v>0.27</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="5" t="s">
         <v>5</v>
       </c>
       <c r="E14" s="13">
-        <v>0.71899999999999997</v>
+        <v>0.28100000000000003</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -1555,28 +1608,36 @@
         <v>7</v>
       </c>
       <c r="B15" s="14">
-        <v>4.7E-2</v>
+        <v>0.65800000000000003</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="9" t="s">
         <v>7</v>
       </c>
       <c r="E15" s="14">
-        <v>0.95</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="15.6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="G17" s="1"/>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="G18" s="1"/>
+      <c r="I18" s="20"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B19" s="12"/>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B20" s="13"/>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21" s="13"/>
     </row>
   </sheetData>

</xml_diff>